<commit_message>
Fix issue of HService
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/oob/data/admin.authority.xlsx
+++ b/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/oob/data/admin.authority.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/zero-cloud/vertx-zero/vertx-pin/zero-rbac/src/main/resources/plugin/rbac/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96F66C5-9E7D-7047-9D54-DE886C13B9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B547725-9A2B-844A-A363-10D6B75906C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="10000" windowWidth="38400" windowHeight="12560" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="71">
   <si>
     <t>key</t>
   </si>
@@ -302,6 +302,10 @@
   </si>
   <si>
     <t>ROLE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>io.vertx.aeon.specification.secure.HSUiNorm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -959,7 +963,7 @@
   <dimension ref="A3:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18"/>
@@ -970,7 +974,7 @@
     <col min="4" max="4" width="11.33203125" style="30" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" style="21" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13.83203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="31" customWidth="1"/>
     <col min="11" max="11" width="13" style="31" bestFit="1" customWidth="1"/>
@@ -1121,7 +1125,9 @@
         <v>11</v>
       </c>
       <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="H6" s="28" t="s">
+        <v>70</v>
+      </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
       <c r="K6" s="29" t="s">

</xml_diff>